<commit_message>
cleaned up data imports to prevent redundant loads
added motor component with efficiency torque/rpm map
</commit_message>
<xml_diff>
--- a/openconcept/propulsion/empirical_data/H3X_HPDM_2300_eff.xlsx
+++ b/openconcept/propulsion/empirical_data/H3X_HPDM_2300_eff.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eosaircraft-my.sharepoint.com/personal/aamos_eos_aero/Documents/Documents/GitHub/openconcept/openconcept/propulsion/empirical_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="8_{A8DC8043-93FE-428E-B915-CB1CDDC91C4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D09C74EC-A4BB-4ACB-88CF-521F02B7D592}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="8_{A8DC8043-93FE-428E-B915-CB1CDDC91C4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2597FB68-F753-4389-BFEE-4E31A077BEC9}"/>
   <bookViews>
-    <workbookView xWindow="-16200" yWindow="2850" windowWidth="28770" windowHeight="16890" xr2:uid="{6CDB121E-BC31-4B8D-9E35-C82BE1F2703E}"/>
+    <workbookView xWindow="29580" yWindow="780" windowWidth="21600" windowHeight="12585" xr2:uid="{6CDB121E-BC31-4B8D-9E35-C82BE1F2703E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -97,6 +97,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -422,9 +426,12 @@
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -435,7 +442,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>986.84210526315803</v>
       </c>
@@ -446,7 +453,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>951.75438596491199</v>
       </c>
@@ -457,7 +464,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>916.66666666666697</v>
       </c>
@@ -468,7 +475,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>877.19298245614004</v>
       </c>
@@ -479,7 +486,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>850.87719298245599</v>
       </c>
@@ -490,7 +497,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>802.63157894736798</v>
       </c>
@@ -501,7 +508,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>763.15789473684197</v>
       </c>
@@ -512,7 +519,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>692.98245614035</v>
       </c>
@@ -523,7 +530,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>649.12280701754298</v>
       </c>
@@ -534,7 +541,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>614.03508771929796</v>
       </c>
@@ -545,7 +552,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>587.71929824561403</v>
       </c>
@@ -556,7 +563,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>552.63157894736798</v>
       </c>
@@ -567,7 +574,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>526.31578947368405</v>
       </c>
@@ -578,7 +585,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>495.614035087719</v>
       </c>
@@ -589,7 +596,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>464.91228070175401</v>
       </c>
@@ -600,7 +607,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>429.82456140350803</v>
       </c>
@@ -611,7 +618,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>403.50877192982398</v>
       </c>
@@ -622,7 +629,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>385.96491228070101</v>
       </c>
@@ -633,7 +640,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>368.42105263157902</v>
       </c>
@@ -644,7 +651,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>355.26315789473699</v>
       </c>
@@ -655,7 +662,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>342.105263157894</v>
       </c>
@@ -666,7 +673,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>342.105263157894</v>
       </c>
@@ -677,7 +684,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>350.87719298245599</v>
       </c>
@@ -688,7 +695,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>368.42105263157799</v>
       </c>
@@ -699,7 +706,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>399.12280701754298</v>
       </c>
@@ -710,7 +717,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>456.14035087719299</v>
       </c>
@@ -721,7 +728,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>526.31578947368405</v>
       </c>
@@ -732,7 +739,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>627.19298245614004</v>
       </c>
@@ -743,7 +750,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>723.68421052631504</v>
       </c>
@@ -754,7 +761,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>807.01754385964796</v>
       </c>
@@ -765,7 +772,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>903.50877192982398</v>
       </c>
@@ -776,7 +783,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>986.84210526315701</v>
       </c>
@@ -787,7 +794,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>1083.3333333333301</v>
       </c>
@@ -798,7 +805,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>1179.8245614035</v>
       </c>
@@ -809,7 +816,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>1302.6315789473599</v>
       </c>
@@ -820,7 +827,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>1394.7368421052599</v>
       </c>
@@ -831,7 +838,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>1464.91228070175</v>
       </c>
@@ -842,7 +849,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>1605.2631578947301</v>
       </c>
@@ -853,7 +860,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>1713.45029239766</v>
       </c>
@@ -864,7 +871,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>1785.08771929824</v>
       </c>
@@ -875,7 +882,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>1118.4210526315701</v>
       </c>
@@ -886,7 +893,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>1061.4035087719301</v>
       </c>
@@ -897,7 +904,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>1013.15789473684</v>
       </c>
@@ -908,7 +915,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>973.68421052631595</v>
       </c>
@@ -919,7 +926,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>938.59649122807002</v>
       </c>
@@ -930,7 +937,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>885.96491228070204</v>
       </c>
@@ -941,7 +948,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>833.33333333333303</v>
       </c>
@@ -952,7 +959,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>798.24561403508699</v>
       </c>
@@ -963,7 +970,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>758.77192982456097</v>
       </c>
@@ -974,7 +981,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>723.68421052631504</v>
       </c>
@@ -985,7 +992,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>692.98245614035</v>
       </c>
@@ -996,7 +1003,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>657.89473684210498</v>
       </c>
@@ -1007,7 +1014,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>622.80701754385905</v>
       </c>
@@ -1018,7 +1025,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>596.491228070175</v>
       </c>
@@ -1029,7 +1036,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>570.17543859649095</v>
       </c>
@@ -1040,7 +1047,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>543.85964912280701</v>
       </c>
@@ -1051,7 +1058,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>517.54385964912206</v>
       </c>
@@ -1062,7 +1069,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>491.22807017543801</v>
       </c>
@@ -1073,7 +1080,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>447.36842105263099</v>
       </c>
@@ -1084,7 +1091,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>421.052631578947</v>
       </c>
@@ -1095,7 +1102,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>403.50877192982398</v>
       </c>
@@ -1106,7 +1113,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>385.96491228070101</v>
       </c>
@@ -1117,7 +1124,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>394.73684210526301</v>
       </c>
@@ -1128,7 +1135,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>412.28070175438501</v>
       </c>
@@ -1139,7 +1146,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>456.14035087719299</v>
       </c>
@@ -1150,7 +1157,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>530.70175438596402</v>
       </c>
@@ -1161,7 +1168,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>592.105263157894</v>
       </c>
@@ -1172,7 +1179,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>701.75438596491199</v>
       </c>
@@ -1183,7 +1190,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>859.64912280701697</v>
       </c>
@@ -1194,7 +1201,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>973.68421052631504</v>
       </c>
@@ -1205,7 +1212,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>1078.94736842105</v>
       </c>
@@ -1216,7 +1223,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>1197.3684210526301</v>
       </c>
@@ -1227,7 +1234,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>1359.6491228070099</v>
       </c>
@@ -1238,7 +1245,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>1456.14035087719</v>
       </c>
@@ -1249,7 +1256,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>1543.8596491228</v>
       </c>
@@ -1260,7 +1267,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>1657.8947368421</v>
       </c>
@@ -1271,7 +1278,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>1728.07017543859</v>
       </c>
@@ -1282,7 +1289,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>1276.3157894736801</v>
       </c>
@@ -1293,7 +1300,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>1236.84210526315</v>
       </c>
@@ -1304,7 +1311,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>1192.98245614035</v>
       </c>
@@ -1315,7 +1322,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>1149.12280701754</v>
       </c>
@@ -1326,7 +1333,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>1096.4912280701701</v>
       </c>
@@ -1337,7 +1344,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>1035.08771929824</v>
       </c>
@@ -1348,7 +1355,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>995.614035087719</v>
       </c>
@@ -1359,7 +1366,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>956.14035087719299</v>
       </c>
@@ -1370,7 +1377,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>894.73684210526301</v>
       </c>
@@ -1381,7 +1388,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>846.491228070175</v>
       </c>
@@ -1392,7 +1399,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>802.63157894736798</v>
       </c>
@@ -1403,7 +1410,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>758.77192982456097</v>
       </c>
@@ -1414,7 +1421,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>710.52631578947296</v>
       </c>
@@ -1425,7 +1432,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>675.43859649122805</v>
       </c>
@@ -1436,7 +1443,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>635.96491228070101</v>
       </c>
@@ -1447,7 +1454,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>596.491228070175</v>
       </c>
@@ -1458,7 +1465,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>570.17543859649095</v>
       </c>
@@ -1469,7 +1476,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>543.85964912280701</v>
       </c>
@@ -1480,7 +1487,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>508.77192982456103</v>
       </c>
@@ -1491,7 +1498,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>482.45614035087698</v>
       </c>
@@ -1502,7 +1509,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>460.52631578947302</v>
       </c>
@@ -1513,7 +1520,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>447.36842105263099</v>
       </c>
@@ -1524,7 +1531,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>442.98245614035</v>
       </c>
@@ -1535,7 +1542,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>456.14035087719299</v>
       </c>
@@ -1546,7 +1553,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>482.45614035087698</v>
       </c>
@@ -1557,7 +1564,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>539.47368421052602</v>
       </c>
@@ -1568,7 +1575,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>631.57894736842104</v>
       </c>
@@ -1579,7 +1586,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>723.68421052631504</v>
       </c>
@@ -1590,7 +1597,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>802.63157894736798</v>
       </c>
@@ -1601,7 +1608,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>872.80701754385905</v>
       </c>
@@ -1612,7 +1619,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>947.36842105263099</v>
       </c>
@@ -1623,7 +1630,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>1043.8596491228</v>
       </c>
@@ -1634,7 +1641,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>1144.7368421052599</v>
       </c>
@@ -1645,7 +1652,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>1263.15789473684</v>
       </c>
@@ -1656,7 +1663,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>1377.19298245614</v>
       </c>
@@ -1667,7 +1674,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>1478.07017543859</v>
       </c>
@@ -1678,7 +1685,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>1578.94736842105</v>
       </c>
@@ -1689,7 +1696,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>1666.6666666666599</v>
       </c>
@@ -1700,7 +1707,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>1723.6842105263099</v>
       </c>
@@ -1711,7 +1718,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>1491.22807017543</v>
       </c>
@@ -1722,7 +1729,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>1464.91228070175</v>
       </c>
@@ -1733,7 +1740,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>1421.05263157894</v>
       </c>
@@ -1744,7 +1751,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>1368.4210526315701</v>
       </c>
@@ -1755,7 +1762,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>1337.7192982456099</v>
       </c>
@@ -1766,7 +1773,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>1280.7017543859599</v>
       </c>
@@ -1777,7 +1784,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>1236.84210526315</v>
       </c>
@@ -1788,7 +1795,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>1201.7543859649099</v>
       </c>
@@ -1799,7 +1806,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>1166.6666666666599</v>
       </c>
@@ -1810,7 +1817,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>1131.5789473684199</v>
       </c>
@@ -1821,7 +1828,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>1083.3333333333301</v>
       </c>
@@ -1832,7 +1839,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>1026.3157894736801</v>
       </c>
@@ -1843,7 +1850,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>991.22807017543801</v>
       </c>
@@ -1854,7 +1861,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>934.21052631578902</v>
       </c>
@@ -1865,7 +1872,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>894.73684210526301</v>
       </c>
@@ -1876,7 +1883,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>859.64912280701697</v>
       </c>
@@ -1887,7 +1894,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>820.17543859649095</v>
       </c>
@@ -1898,7 +1905,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>776.31578947368405</v>
       </c>
@@ -1909,7 +1916,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>728.07017543859604</v>
       </c>
@@ -1920,7 +1927,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>675.43859649122805</v>
       </c>
@@ -1931,7 +1938,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>640.35087719298201</v>
       </c>
@@ -1942,7 +1949,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>609.64912280701697</v>
       </c>
@@ -1953,7 +1960,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>574.56140350877195</v>
       </c>
@@ -1964,7 +1971,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>552.63157894736798</v>
       </c>
@@ -1975,7 +1982,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>530.70175438596402</v>
       </c>
@@ -1986,7 +1993,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>517.54385964912206</v>
       </c>
@@ -1997,7 +2004,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>526.31578947368405</v>
       </c>
@@ -2008,7 +2015,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>561.40350877192895</v>
       </c>
@@ -2019,7 +2026,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>614.03508771929796</v>
       </c>
@@ -2030,7 +2037,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>679.82456140350803</v>
       </c>
@@ -2041,7 +2048,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>745.614035087719</v>
       </c>
@@ -2052,7 +2059,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>820.17543859649095</v>
       </c>
@@ -2063,7 +2070,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>890.35087719298201</v>
       </c>
@@ -2074,7 +2081,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>973.68421052631504</v>
       </c>
@@ -2085,7 +2092,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>1043.8596491228</v>
       </c>
@@ -2096,7 +2103,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>1122.80701754385</v>
       </c>
@@ -2107,7 +2114,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>1210.5263157894699</v>
       </c>
@@ -2118,7 +2125,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>1293.8596491228</v>
       </c>
@@ -2129,7 +2136,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>1399.12280701754</v>
       </c>
@@ -2140,7 +2147,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>1495.6140350877099</v>
       </c>
@@ -2151,7 +2158,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>1605.2631578947301</v>
       </c>
@@ -2162,7 +2169,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>1684.21052631578</v>
       </c>
@@ -2173,7 +2180,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>1736.84210526315</v>
       </c>
@@ -2184,7 +2191,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>846.491228070175</v>
       </c>
@@ -2195,7 +2202,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>885.96491228070101</v>
       </c>
@@ -2206,7 +2213,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>925.43859649122805</v>
       </c>
@@ -2217,7 +2224,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>964.91228070175396</v>
       </c>
@@ -2228,7 +2235,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>991.22807017543801</v>
       </c>
@@ -2239,7 +2246,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>1030.7017543859599</v>
       </c>
@@ -2250,7 +2257,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>1074.5614035087699</v>
       </c>
@@ -2261,7 +2268,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>1131.5789473684199</v>
       </c>
@@ -2272,7 +2279,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>1166.6666666666599</v>
       </c>
@@ -2283,7 +2290,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>1223.6842105263099</v>
       </c>
@@ -2294,7 +2301,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>1293.8596491228</v>
       </c>
@@ -2305,7 +2312,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>1377.19298245614</v>
       </c>
@@ -2316,7 +2323,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>1429.8245614035</v>
       </c>
@@ -2327,7 +2334,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>1482.4561403508701</v>
       </c>
@@ -2338,7 +2345,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>1526.3157894736801</v>
       </c>
@@ -2349,7 +2356,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>1570.17543859649</v>
       </c>
@@ -2360,7 +2367,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>1631.5789473684199</v>
       </c>
@@ -2371,7 +2378,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>1701.7543859649099</v>
       </c>
@@ -2382,7 +2389,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>1749.99999999999</v>
       </c>
@@ -2393,7 +2400,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>1785.08771929824</v>
       </c>
@@ -2404,7 +2411,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>815.78947368420995</v>
       </c>
@@ -2415,7 +2422,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>780.70175438596402</v>
       </c>
@@ -2426,7 +2433,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>745.614035087719</v>
       </c>
@@ -2437,7 +2444,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>710.52631578947296</v>
       </c>
@@ -2448,7 +2455,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>675.43859649122805</v>
       </c>
@@ -2459,7 +2466,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>657.89473684210498</v>
       </c>
@@ -2470,7 +2477,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>644.73684210526301</v>
       </c>
@@ -2481,7 +2488,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>635.96491228070101</v>
       </c>
@@ -2492,7 +2499,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>640.35087719298201</v>
       </c>
@@ -2503,7 +2510,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>644.73684210526301</v>
       </c>
@@ -2514,7 +2521,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>653.50877192982398</v>
       </c>
@@ -2525,7 +2532,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>679.82456140350803</v>
       </c>
@@ -2536,7 +2543,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>697.36842105263099</v>
       </c>
@@ -2547,7 +2554,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>714.91228070175396</v>
       </c>
@@ -2558,7 +2565,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>728.07017543859604</v>
       </c>
@@ -2569,7 +2576,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>745.614035087719</v>
       </c>
@@ -2580,7 +2587,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>771.92982456140305</v>
       </c>
@@ -2591,7 +2598,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198">
         <v>793.85964912280701</v>
       </c>
@@ -2602,7 +2609,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199">
         <v>811.40350877192895</v>
       </c>
@@ -2613,7 +2620,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200">
         <v>837.71929824561403</v>
       </c>
@@ -2624,7 +2631,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A201">
         <v>864.03508771929796</v>
       </c>
@@ -2635,7 +2642,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A202">
         <v>881.57894736842104</v>
       </c>
@@ -2646,7 +2653,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A203">
         <v>903.50877192982398</v>
       </c>
@@ -2657,7 +2664,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A204">
         <v>929.82456140350803</v>
       </c>
@@ -2668,7 +2675,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A205">
         <v>956.14035087719299</v>
       </c>
@@ -2679,7 +2686,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A206">
         <v>995.614035087719</v>
       </c>
@@ -2690,7 +2697,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A207">
         <v>1030.7017543859599</v>
       </c>
@@ -2701,7 +2708,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A208">
         <v>1070.17543859649</v>
       </c>
@@ -2712,7 +2719,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A209">
         <v>1105.2631578947301</v>
       </c>
@@ -2723,7 +2730,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A210">
         <v>1144.7368421052599</v>
       </c>
@@ -2734,7 +2741,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A211">
         <v>1197.3684210526301</v>
       </c>
@@ -2745,7 +2752,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A212">
         <v>1241.22807017543</v>
       </c>
@@ -2756,7 +2763,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A213">
         <v>1285.08771929824</v>
       </c>
@@ -2767,7 +2774,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A214">
         <v>1315.78947368421</v>
       </c>
@@ -2778,7 +2785,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A215">
         <v>1359.6491228070099</v>
       </c>
@@ -2789,7 +2796,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A216">
         <v>1394.7368421052599</v>
       </c>
@@ -2800,7 +2807,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A217">
         <v>1447.3684210526301</v>
       </c>
@@ -2811,7 +2818,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A218">
         <v>1486.84210526315</v>
       </c>
@@ -2822,7 +2829,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A219">
         <v>1535.08771929824</v>
       </c>
@@ -2833,7 +2840,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A220">
         <v>1587.7192982456099</v>
       </c>
@@ -2844,7 +2851,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A221">
         <v>1635.9649122807</v>
       </c>
@@ -2855,7 +2862,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A222">
         <v>1671.05263157894</v>
       </c>
@@ -2866,7 +2873,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A223">
         <v>1719.2982456140301</v>
       </c>
@@ -2877,7 +2884,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A224">
         <v>1758.7719298245599</v>
       </c>
@@ -2888,7 +2895,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A225">
         <v>1798.2456140350801</v>
       </c>
@@ -2899,7 +2906,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A226">
         <v>1789.473684</v>
       </c>
@@ -2910,7 +2917,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A227">
         <v>1728.0701750000001</v>
       </c>
@@ -2921,7 +2928,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A228">
         <v>1644.736842</v>
       </c>
@@ -2932,7 +2939,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A229">
         <v>1530.7017539999999</v>
       </c>
@@ -2943,7 +2950,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A230">
         <v>1438.596491</v>
       </c>
@@ -2954,7 +2961,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A231">
         <v>1381.578947</v>
       </c>
@@ -2965,7 +2972,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A232">
         <v>1337.719298</v>
       </c>
@@ -2976,7 +2983,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A233">
         <v>1280.7017539999999</v>
       </c>
@@ -2987,7 +2994,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A234">
         <v>1250</v>
       </c>
@@ -2998,7 +3005,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A235">
         <v>1175.438596</v>
       </c>
@@ -3009,7 +3016,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="236" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A236">
         <v>1122.807018</v>
       </c>
@@ -3020,7 +3027,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A237">
         <v>1078.9473680000001</v>
       </c>
@@ -3031,7 +3038,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A238">
         <v>1021.9298250000001</v>
       </c>
@@ -3042,7 +3049,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="239" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A239">
         <v>973.68421049999995</v>
       </c>
@@ -3053,7 +3060,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A240">
         <v>925.43859650000002</v>
       </c>
@@ -3064,7 +3071,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A241">
         <v>885.96491230000004</v>
       </c>
@@ -3075,7 +3082,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A242">
         <v>842.10526319999997</v>
       </c>
@@ -3086,7 +3093,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A243">
         <v>837.71929820000003</v>
       </c>
@@ -3097,7 +3104,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A244">
         <v>833.33333330000005</v>
       </c>
@@ -3108,7 +3115,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="245" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A245">
         <v>842.10526319999997</v>
       </c>
@@ -3119,7 +3126,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A246">
         <v>859.64912279999999</v>
       </c>
@@ -3130,7 +3137,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="247" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A247">
         <v>881.57894739999995</v>
       </c>
@@ -3141,7 +3148,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="248" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A248">
         <v>907.89473680000003</v>
       </c>
@@ -3152,7 +3159,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="249" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A249">
         <v>925.43859650000002</v>
       </c>
@@ -3163,7 +3170,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A250">
         <v>947.36842109999998</v>
       </c>
@@ -3174,7 +3181,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="251" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A251">
         <v>982.45614039999998</v>
       </c>
@@ -3185,7 +3192,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A252">
         <v>1008.77193</v>
       </c>
@@ -3196,7 +3203,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="253" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A253">
         <v>1048.2456139999999</v>
       </c>
@@ -3207,7 +3214,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="254" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A254">
         <v>1087.719298</v>
       </c>
@@ -3218,7 +3225,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="255" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A255">
         <v>1131.578947</v>
       </c>
@@ -3229,7 +3236,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="256" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A256">
         <v>1175.438596</v>
       </c>
@@ -3240,7 +3247,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="257" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A257">
         <v>1201.7543860000001</v>
       </c>
@@ -3251,7 +3258,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="258" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A258">
         <v>1236.8421049999999</v>
       </c>
@@ -3262,7 +3269,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="259" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A259">
         <v>1263.1578950000001</v>
       </c>
@@ -3273,7 +3280,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="260" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A260">
         <v>1320.1754390000001</v>
       </c>
@@ -3284,7 +3291,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="261" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A261">
         <v>1364.0350880000001</v>
       </c>
@@ -3295,7 +3302,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="262" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A262">
         <v>1407.8947370000001</v>
       </c>
@@ -3306,7 +3313,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="263" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A263">
         <v>1456.140351</v>
       </c>
@@ -3317,7 +3324,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="264" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A264">
         <v>1495.6140350000001</v>
       </c>
@@ -3328,7 +3335,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="265" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A265">
         <v>1539.473684</v>
       </c>
@@ -3339,7 +3346,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="266" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A266">
         <v>1574.561404</v>
       </c>
@@ -3350,7 +3357,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="267" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A267">
         <v>1635.9649119999999</v>
       </c>
@@ -3361,7 +3368,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="268" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A268">
         <v>1675.438596</v>
       </c>
@@ -3372,7 +3379,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="269" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A269">
         <v>1723.684211</v>
       </c>
@@ -3383,7 +3390,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="270" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A270">
         <v>1789.473684</v>
       </c>
@@ -3394,7 +3401,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="271" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A271">
         <v>1780.7017539999999</v>
       </c>
@@ -3405,7 +3412,7 @@
         <v>0.96</v>
       </c>
     </row>
-    <row r="272" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A272">
         <v>1741.2280699999999</v>
       </c>
@@ -3416,7 +3423,7 @@
         <v>0.96</v>
       </c>
     </row>
-    <row r="273" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A273">
         <v>1688.596491</v>
       </c>
@@ -3427,7 +3434,7 @@
         <v>0.96</v>
       </c>
     </row>
-    <row r="274" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A274">
         <v>1618.421053</v>
       </c>
@@ -3438,7 +3445,7 @@
         <v>0.96</v>
       </c>
     </row>
-    <row r="275" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A275">
         <v>1552.6315790000001</v>
       </c>
@@ -3449,7 +3456,7 @@
         <v>0.96</v>
       </c>
     </row>
-    <row r="276" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A276">
         <v>1469.2982460000001</v>
       </c>
@@ -3460,7 +3467,7 @@
         <v>0.96</v>
       </c>
     </row>
-    <row r="277" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A277">
         <v>1403.5087719999999</v>
       </c>
@@ -3471,7 +3478,7 @@
         <v>0.96</v>
       </c>
     </row>
-    <row r="278" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A278">
         <v>1368.421053</v>
       </c>
@@ -3482,7 +3489,7 @@
         <v>0.96</v>
       </c>
     </row>
-    <row r="279" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A279">
         <v>1333.333333</v>
       </c>
@@ -3493,7 +3500,7 @@
         <v>0.96</v>
       </c>
     </row>
-    <row r="280" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A280">
         <v>1302.6315790000001</v>
       </c>
@@ -3504,7 +3511,7 @@
         <v>0.96</v>
       </c>
     </row>
-    <row r="281" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A281">
         <v>1263.1578950000001</v>
       </c>
@@ -3515,7 +3522,7 @@
         <v>0.96</v>
       </c>
     </row>
-    <row r="282" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A282">
         <v>1236.8421049999999</v>
       </c>
@@ -3526,7 +3533,7 @@
         <v>0.96</v>
       </c>
     </row>
-    <row r="283" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A283">
         <v>1210.526316</v>
       </c>
@@ -3537,7 +3544,7 @@
         <v>0.96</v>
       </c>
     </row>
-    <row r="284" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A284">
         <v>1188.596491</v>
       </c>
@@ -3548,7 +3555,7 @@
         <v>0.96</v>
       </c>
     </row>
-    <row r="285" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A285">
         <v>1184.2105260000001</v>
       </c>
@@ -3559,7 +3566,7 @@
         <v>0.96</v>
       </c>
     </row>
-    <row r="286" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A286">
         <v>1192.982456</v>
       </c>
@@ -3570,7 +3577,7 @@
         <v>0.96</v>
       </c>
     </row>
-    <row r="287" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A287">
         <v>1210.526316</v>
       </c>
@@ -3581,7 +3588,7 @@
         <v>0.96</v>
       </c>
     </row>
-    <row r="288" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A288">
         <v>1228.0701750000001</v>
       </c>
@@ -3592,7 +3599,7 @@
         <v>0.96</v>
       </c>
     </row>
-    <row r="289" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="289" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A289">
         <v>1263.1578950000001</v>
       </c>
@@ -3603,7 +3610,7 @@
         <v>0.96</v>
       </c>
     </row>
-    <row r="290" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A290">
         <v>1289.473684</v>
       </c>
@@ -3614,7 +3621,7 @@
         <v>0.96</v>
       </c>
     </row>
-    <row r="291" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="291" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A291">
         <v>1315.7894739999999</v>
       </c>
@@ -3625,7 +3632,7 @@
         <v>0.96</v>
       </c>
     </row>
-    <row r="292" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="292" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A292">
         <v>1342.1052629999999</v>
       </c>
@@ -3636,7 +3643,7 @@
         <v>0.96</v>
       </c>
     </row>
-    <row r="293" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="293" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A293">
         <v>1372.807018</v>
       </c>
@@ -3647,7 +3654,7 @@
         <v>0.96</v>
       </c>
     </row>
-    <row r="294" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="294" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A294">
         <v>1407.8947370000001</v>
       </c>
@@ -3658,7 +3665,7 @@
         <v>0.96</v>
       </c>
     </row>
-    <row r="295" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="295" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A295">
         <v>1438.596491</v>
       </c>
@@ -3669,7 +3676,7 @@
         <v>0.96</v>
       </c>
     </row>
-    <row r="296" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="296" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A296">
         <v>1478.0701750000001</v>
       </c>
@@ -3680,7 +3687,7 @@
         <v>0.96</v>
       </c>
     </row>
-    <row r="297" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="297" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A297">
         <v>1517.54386</v>
       </c>
@@ -3691,7 +3698,7 @@
         <v>0.96</v>
       </c>
     </row>
-    <row r="298" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="298" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A298">
         <v>1552.6315790000001</v>
       </c>
@@ -3702,7 +3709,7 @@
         <v>0.96</v>
       </c>
     </row>
-    <row r="299" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="299" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A299">
         <v>1587.719298</v>
       </c>
@@ -3713,7 +3720,7 @@
         <v>0.96</v>
       </c>
     </row>
-    <row r="300" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="300" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A300">
         <v>1657.8947370000001</v>
       </c>
@@ -3724,7 +3731,7 @@
         <v>0.96</v>
       </c>
     </row>
-    <row r="301" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="301" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A301">
         <v>1719.2982460000001</v>
       </c>
@@ -3735,7 +3742,7 @@
         <v>0.96</v>
       </c>
     </row>
-    <row r="302" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="302" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A302">
         <v>1758.7719300000001</v>
       </c>
@@ -3746,7 +3753,7 @@
         <v>0.96</v>
       </c>
     </row>
-    <row r="303" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="303" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A303">
         <v>1798.2456139999999</v>
       </c>

</xml_diff>